<commit_message>
Commit after example recording for Lab data cleaning steps
</commit_message>
<xml_diff>
--- a/hrs/G2A HRS Longitudinal Variable List.xlsx
+++ b/hrs/G2A HRS Longitudinal Variable List.xlsx
@@ -3,19 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D17F9B-036E-4E55-88C1-D3C55AE4C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693C204F-C504-4AB2-85C9-3AA8F29B7A1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-15210" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3210" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wave8" sheetId="14" r:id="rId1"/>
-    <sheet name="wave9" sheetId="12" r:id="rId2"/>
-    <sheet name="wave10" sheetId="13" r:id="rId3"/>
-    <sheet name="wave11" sheetId="11" r:id="rId4"/>
-    <sheet name="wave12" sheetId="10" r:id="rId5"/>
-    <sheet name="wave13" sheetId="8" r:id="rId6"/>
-    <sheet name="wave14" sheetId="9" r:id="rId7"/>
-    <sheet name="household" sheetId="7" r:id="rId8"/>
+    <sheet name="biomarker" sheetId="15" r:id="rId2"/>
+    <sheet name="wave9" sheetId="12" r:id="rId3"/>
+    <sheet name="wave10" sheetId="13" r:id="rId4"/>
+    <sheet name="wave11" sheetId="11" r:id="rId5"/>
+    <sheet name="wave12" sheetId="10" r:id="rId6"/>
+    <sheet name="wave13" sheetId="8" r:id="rId7"/>
+    <sheet name="wave14" sheetId="9" r:id="rId8"/>
+    <sheet name="household" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2051" uniqueCount="606">
   <si>
     <t>BMI</t>
   </si>
@@ -1794,6 +1795,57 @@
   </si>
   <si>
     <t>S8MSTAT</t>
+  </si>
+  <si>
+    <t>RAEHSAMP</t>
+  </si>
+  <si>
+    <t>A1C BIOSAFE</t>
+  </si>
+  <si>
+    <t>a1cbios</t>
+  </si>
+  <si>
+    <t>wave6</t>
+  </si>
+  <si>
+    <t>wave8</t>
+  </si>
+  <si>
+    <t>LA1CBIOS</t>
+  </si>
+  <si>
+    <t>KA1CBIOS</t>
+  </si>
+  <si>
+    <t>KA1C_ADJ</t>
+  </si>
+  <si>
+    <t>a1c_adj</t>
+  </si>
+  <si>
+    <t>KAHDLBIOS</t>
+  </si>
+  <si>
+    <t>ahdlbios</t>
+  </si>
+  <si>
+    <t>HDL BIOSAFE</t>
+  </si>
+  <si>
+    <t>NHANES EQUIVALENT A1C</t>
+  </si>
+  <si>
+    <t>wave10</t>
+  </si>
+  <si>
+    <t>wave12</t>
+  </si>
+  <si>
+    <t>wave14</t>
+  </si>
+  <si>
+    <t>wave16</t>
   </si>
 </sst>
 </file>
@@ -1859,7 +1911,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2348,12 +2410,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10186C6F-BDD5-4582-A081-8CCA034FDB9F}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection activeCell="D52" sqref="D52"/>
       <selection pane="topRight" activeCell="D52" sqref="D52"/>
       <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52:E52"/>
+      <selection pane="bottomRight" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2424,8 +2486,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="D3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E3" t="s">
+        <v>589</v>
+      </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
@@ -3377,13 +3443,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B69:B1048576 B54:B64 B1">
-    <cfRule type="duplicateValues" dxfId="20" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57 H47:I47 F1 H46 H48:H56 F59:F1048576">
-    <cfRule type="duplicateValues" dxfId="19" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G1048576 I46:I56 D57:E1048576 G1 D1:E1">
-    <cfRule type="duplicateValues" dxfId="18" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3391,15 +3457,131 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35A90E4A-1390-4FAC-90BE-D7C204CE5173}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>592</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>602</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>603</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>590</v>
+      </c>
+      <c r="C4" t="s">
+        <v>591</v>
+      </c>
+      <c r="D4" t="s">
+        <v>595</v>
+      </c>
+      <c r="E4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>601</v>
+      </c>
+      <c r="C5" t="s">
+        <v>597</v>
+      </c>
+      <c r="D5" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>600</v>
+      </c>
+      <c r="C6" t="s">
+        <v>599</v>
+      </c>
+      <c r="D6" t="s">
+        <v>598</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402DEB4F-F9A8-4998-83EB-DEA9A79D2A12}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D52" sqref="D52"/>
-      <selection pane="topRight" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52:E52"/>
+      <selection activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3470,8 +3652,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="D3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E3" t="s">
+        <v>589</v>
+      </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
@@ -4423,29 +4609,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B69:B1048576 B54:B64 B1">
-    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57 H47:I47 F1 H46 H48:H56 F59:F1048576">
-    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G1048576 I46:I56 D57:E1048576 G1 D1:E1">
-    <cfRule type="duplicateValues" dxfId="15" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90DB33B7-BCD3-4D28-AC39-7800AC56B343}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D52" sqref="D52"/>
-      <selection pane="topRight" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52:E52"/>
+      <selection activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4516,8 +4702,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="D3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E3" t="s">
+        <v>589</v>
+      </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
@@ -5469,29 +5659,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B69:B1048576 B54:B64 B1">
-    <cfRule type="duplicateValues" dxfId="14" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57 H47:I47 F1 H46 H48:H56 F59:F1048576">
-    <cfRule type="duplicateValues" dxfId="13" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G1048576 I46:I56 D57:E1048576 G1 D1:E1">
-    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B5DC06-3C98-4C0D-AB4D-188AF125BA6B}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D52" sqref="D52"/>
-      <selection pane="topRight" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52:E52"/>
+      <selection activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5562,8 +5752,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="D3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E3" t="s">
+        <v>589</v>
+      </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
@@ -6515,29 +6709,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B69:B1048576 B54:B64 B1">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57 H47:I47 F1 H46 H48:H56 F59:F1048576">
-    <cfRule type="duplicateValues" dxfId="10" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G1048576 I46:I56 D57:E1048576 G1 D1:E1">
-    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581D3D43-A935-4EC9-86EC-C8C3944D3E11}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D52" sqref="D52"/>
-      <selection pane="topRight" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52:E52"/>
+      <selection activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6608,8 +6802,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="D3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E3" t="s">
+        <v>589</v>
+      </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
@@ -7561,29 +7759,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B69:B1048576 B54:B64 B1">
-    <cfRule type="duplicateValues" dxfId="8" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57 H47:I47 F1 H46 H48:H56 F59:F1048576">
-    <cfRule type="duplicateValues" dxfId="7" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G1048576 I46:I56 D57:E1048576 G1 D1:E1">
-    <cfRule type="duplicateValues" dxfId="6" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1149310-DFBD-437B-AA38-15E3D7623C20}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D52" sqref="D52"/>
-      <selection pane="topRight" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52:E52"/>
+      <selection activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7654,8 +7852,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="D3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E3" t="s">
+        <v>589</v>
+      </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
@@ -8607,29 +8809,29 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B69:B1048576 B54:B64 B1">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57 H47:I47 F1 H46 H48:H56 F59:F1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G1048576 I46:I56 D57:E1048576 G1 D1:E1">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{209F2E6C-4F17-4ED0-8D83-63A50DE26C70}">
   <dimension ref="A1:I58"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="D52" sqref="D52"/>
-      <selection pane="topRight" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
-      <selection pane="bottomRight" activeCell="D52" sqref="D52:E52"/>
+      <selection activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8700,8 +8902,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="D3"/>
-      <c r="E3"/>
+      <c r="D3" t="s">
+        <v>589</v>
+      </c>
+      <c r="E3" t="s">
+        <v>589</v>
+      </c>
       <c r="H3" t="s">
         <v>82</v>
       </c>
@@ -9653,20 +9859,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B69:B1048576 B54:B64 B1">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F57 H47:I47 F1 H46 H48:H56 F59:F1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G57:G1048576 I46:I56 D57:E1048576 G1 D1:E1">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{516FB498-DDE8-483E-BF1C-FF0717D5B9F0}">
   <dimension ref="A2:D10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update after cleaning g2aging_falls
</commit_message>
<xml_diff>
--- a/hrs/G2A HRS Longitudinal Variable List.xlsx
+++ b/hrs/G2A HRS Longitudinal Variable List.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBF74C0-A94E-4CC3-8486-5A5D333B861F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09013204-5CC5-44DF-BF13-41160E3B3833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3210" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1785" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wave8" sheetId="14" r:id="rId1"/>
@@ -2428,7 +2428,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2463,12 +2463,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -2762,10 +2756,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4152,7 +4142,7 @@
   <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9346,7 +9336,7 @@
       <selection activeCell="D7" sqref="D7"/>
       <selection pane="topRight" activeCell="D7" sqref="D7"/>
       <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
-      <selection pane="bottomRight" activeCell="C7" sqref="C7"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>